<commit_message>
take Line6 as part of CSM
</commit_message>
<xml_diff>
--- a/BusManagerSecOcDemo.xlsx
+++ b/BusManagerSecOcDemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_XuhuaRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB61EA1-1997-4512-B2C6-277649D0F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A8337C-ABC0-4DB8-8D73-3D4A92B7E622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
   </bookViews>
@@ -7605,8 +7605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38B81CE-79E3-4568-BB50-9E45BADB5D49}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -7674,7 +7674,9 @@
       <c r="B6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="50" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="300" customHeight="1">
       <c r="A7" s="25" t="s">
@@ -7683,9 +7685,7 @@
       <c r="B7" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>105</v>
-      </c>
+      <c r="C7" s="51"/>
     </row>
     <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="25" t="s">
@@ -7889,7 +7889,8 @@
       <c r="C28" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A13:C13"/>

</xml_diff>

<commit_message>
update Line9, how key is generated
</commit_message>
<xml_diff>
--- a/BusManagerSecOcDemo.xlsx
+++ b/BusManagerSecOcDemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_XuhuaRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A8337C-ABC0-4DB8-8D73-3D4A92B7E622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB0D84-8401-4A6A-8176-3E71485F3010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8640" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{EE3554E5-5B85-4F6F-95D2-24E55C4E92D2}"/>
   </bookViews>
@@ -4910,456 +4910,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">char* </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pduSpecificKey</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DsCmacKey_getPduSpecificKey</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>securedIPduName</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>authenticPduName</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UserCode_SecOCHelper_DeriveKeyFromString</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pduSpecificKey</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyPtr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, &amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyLength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DsBusCustomCodeSecOCPduFeature_setKeyPtr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PduFeatureHandle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyPtr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DsBusCustomCodeSecOCPduFeature_setKeyLength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PduFeatureHandle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyLength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UserCode_Csm_KeyElementSet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>featureInstanceData</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CsmJobHandle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRYPTO_KE_MAC_KEY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyPtr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyLength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">caluclating authenticator(Non-truncated)
 </t>
     </r>
@@ -5462,44 +5012,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>freshnessValue</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyPtr</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>keyLength</t>
     </r>
   </si>
   <si>
@@ -6260,6 +5772,585 @@
   </si>
   <si>
     <t>CSM</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">char* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pduSpecificKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DsCmacKey_getPduSpecificKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>securedIPduName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>authenticPduName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserCode_SecOCHelper_DeriveKeyFromString</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pduSpecificKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DsBusCustomCodeSecOCPduFeature_setKeyPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PduFeatureHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DsBusCustomCodeSecOCPduFeature_setKeyLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PduFeatureHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserCode_Csm_KeyElementSet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>featureInstanceData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CsmJobHandle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRYPTO_KE_MAC_KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyPtr</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>keyLength</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+UserCode_Csm_KeyElementSet:
+struct AES_ctx* handle </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DsCmac_newAesCtx() 
+jobHandle-&gt;CTX_Handle </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> handle
+jobHandle-&gt;Crypto_Job-&gt;jobPrimitiveInfo-&gt;cryIfKeyId </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyId
+DsCmac_CMACInit(keyPtr, handle)</t>
+    </r>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
 </sst>
@@ -7605,8 +7696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38B81CE-79E3-4568-BB50-9E45BADB5D49}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -7675,7 +7766,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="300" customHeight="1">
@@ -7683,7 +7774,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" s="51"/>
     </row>
@@ -7695,15 +7786,15 @@
         <v>49</v>
       </c>
       <c r="C8" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="110.1" customHeight="1">
+      <c r="A9" s="27" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="90" customHeight="1">
-      <c r="A9" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>90</v>
+      <c r="B9" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="C9" s="51"/>
     </row>
@@ -7771,7 +7862,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1">
@@ -7816,7 +7907,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="80.099999999999994" customHeight="1">
@@ -7824,7 +7915,7 @@
         <v>84</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="40" t="s">
         <v>83</v>
@@ -7835,10 +7926,10 @@
         <v>85</v>
       </c>
       <c r="B23" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="50" t="s">
         <v>97</v>
-      </c>
-      <c r="C23" s="50" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="90" customHeight="1">
@@ -7846,39 +7937,39 @@
         <v>86</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="51"/>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1">
       <c r="A25" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="110.1" customHeight="1">
       <c r="A26" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="51"/>
     </row>
     <row r="27" spans="1:3" ht="80.099999999999994" customHeight="1">
       <c r="A27" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1">

</xml_diff>